<commit_message>
Added function to reformat excel sheet.
</commit_message>
<xml_diff>
--- a/Assignment4/06222016 Staph Array Data.xlsx
+++ b/Assignment4/06222016 Staph Array Data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28315"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxhaase/Desktop/Grad_School/Fall_2017/Intro_to_programming/Files/Assignment_4/Assignment4/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="6465" activeTab="2"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="17500"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1" sheetId="1" r:id="rId1"/>
@@ -19,8 +24,15 @@
     <sheet name="Plate10" sheetId="10" r:id="rId10"/>
     <sheet name="Plate11" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1769,12 +1781,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1804,12 +1816,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -2015,28 +2027,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB49"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="27" max="27" width="9.140625" customWidth="1"/>
-    <col min="29" max="29" width="8.7109375" customWidth="1"/>
-    <col min="32" max="32" width="13.28515625" customWidth="1"/>
-    <col min="33" max="33" width="13.140625" customWidth="1"/>
-    <col min="45" max="45" width="15.42578125" customWidth="1"/>
-    <col min="46" max="46" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="27" max="27" width="9.1640625" customWidth="1"/>
+    <col min="29" max="29" width="8.6640625" customWidth="1"/>
+    <col min="32" max="32" width="13.33203125" customWidth="1"/>
+    <col min="33" max="33" width="13.1640625" customWidth="1"/>
+    <col min="45" max="45" width="15.5" customWidth="1"/>
+    <col min="46" max="46" width="14.5" customWidth="1"/>
     <col min="47" max="47" width="11" customWidth="1"/>
-    <col min="48" max="48" width="16.140625" customWidth="1"/>
-    <col min="49" max="49" width="11.140625" customWidth="1"/>
+    <col min="48" max="48" width="16.1640625" customWidth="1"/>
+    <col min="49" max="49" width="11.1640625" customWidth="1"/>
     <col min="51" max="51" width="12" customWidth="1"/>
-    <col min="52" max="52" width="13.28515625" customWidth="1"/>
-    <col min="53" max="53" width="18.85546875" customWidth="1"/>
+    <col min="52" max="52" width="13.33203125" customWidth="1"/>
+    <col min="53" max="53" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2048,7 +2060,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:54" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2212,7 +2224,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2364,7 +2376,7 @@
         <v>14945</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2516,7 +2528,7 @@
         <v>18060</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2668,7 +2680,7 @@
         <v>15435</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2820,7 +2832,7 @@
         <v>4918</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2972,7 +2984,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3124,7 +3136,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3276,7 +3288,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
@@ -3437,7 +3449,7 @@
         <v>10981</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3589,7 +3601,7 @@
         <v>4387</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3741,7 +3753,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3893,7 +3905,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>19</v>
       </c>
@@ -4054,7 +4066,7 @@
         <v>11708</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -4206,7 +4218,7 @@
         <v>5186</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -4358,7 +4370,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -4510,7 +4522,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
@@ -4671,7 +4683,7 @@
         <v>16748.25</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>25</v>
       </c>
@@ -4823,7 +4835,7 @@
         <v>15284.5</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>26</v>
       </c>
@@ -4975,7 +4987,7 @@
         <v>5758.5</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>27</v>
       </c>
@@ -5127,7 +5139,7 @@
         <v>831.75</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>28</v>
       </c>
@@ -5288,7 +5300,7 @@
         <v>16753</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>29</v>
       </c>
@@ -5440,7 +5452,7 @@
         <v>18900.75</v>
       </c>
     </row>
-    <row r="24" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>30</v>
       </c>
@@ -5592,7 +5604,7 @@
         <v>7682.75</v>
       </c>
     </row>
-    <row r="25" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>31</v>
       </c>
@@ -5744,7 +5756,7 @@
         <v>1141.5</v>
       </c>
     </row>
-    <row r="26" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>32</v>
       </c>
@@ -5905,7 +5917,7 @@
         <v>18839</v>
       </c>
     </row>
-    <row r="27" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>33</v>
       </c>
@@ -6057,7 +6069,7 @@
         <v>9278</v>
       </c>
     </row>
-    <row r="28" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>34</v>
       </c>
@@ -6209,7 +6221,7 @@
         <v>1662</v>
       </c>
     </row>
-    <row r="29" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>35</v>
       </c>
@@ -6361,7 +6373,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="30" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>36</v>
       </c>
@@ -6522,7 +6534,7 @@
         <v>20336</v>
       </c>
     </row>
-    <row r="31" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>37</v>
       </c>
@@ -6674,7 +6686,7 @@
         <v>12049</v>
       </c>
     </row>
-    <row r="32" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>38</v>
       </c>
@@ -6826,7 +6838,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="33" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>39</v>
       </c>
@@ -6978,7 +6990,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="34" spans="1:53" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:53" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>40</v>
       </c>
@@ -7139,7 +7151,7 @@
         <v>18605</v>
       </c>
     </row>
-    <row r="35" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>41</v>
       </c>
@@ -7291,7 +7303,7 @@
         <v>10447</v>
       </c>
     </row>
-    <row r="36" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>42</v>
       </c>
@@ -7443,7 +7455,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="37" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>43</v>
       </c>
@@ -7595,7 +7607,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="38" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>44</v>
       </c>
@@ -7756,7 +7768,7 @@
         <v>21463</v>
       </c>
     </row>
-    <row r="39" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>45</v>
       </c>
@@ -7908,7 +7920,7 @@
         <v>21901</v>
       </c>
     </row>
-    <row r="40" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>46</v>
       </c>
@@ -8060,7 +8072,7 @@
         <v>8039</v>
       </c>
     </row>
-    <row r="41" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>47</v>
       </c>
@@ -8212,7 +8224,7 @@
         <v>1811</v>
       </c>
     </row>
-    <row r="42" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>48</v>
       </c>
@@ -8373,7 +8385,7 @@
         <v>21520</v>
       </c>
     </row>
-    <row r="43" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>49</v>
       </c>
@@ -8525,7 +8537,7 @@
         <v>16278</v>
       </c>
     </row>
-    <row r="44" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>50</v>
       </c>
@@ -8677,7 +8689,7 @@
         <v>3801</v>
       </c>
     </row>
-    <row r="45" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>51</v>
       </c>
@@ -8829,7 +8841,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="46" spans="1:53" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:53" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>52</v>
       </c>
@@ -8990,7 +9002,7 @@
         <v>20612</v>
       </c>
     </row>
-    <row r="47" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>53</v>
       </c>
@@ -9142,7 +9154,7 @@
         <v>11357</v>
       </c>
     </row>
-    <row r="48" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>54</v>
       </c>
@@ -9294,7 +9306,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="49" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>55</v>
       </c>
@@ -9460,21 +9472,21 @@
       <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="10"/>
-    <col min="15" max="15" width="9.140625" style="10"/>
-    <col min="21" max="21" width="9.140625" style="10"/>
-    <col min="24" max="24" width="9.140625" style="10"/>
-    <col min="30" max="30" width="9.140625" style="10"/>
-    <col min="32" max="32" width="9.140625" style="10"/>
-    <col min="36" max="36" width="9.140625" style="10"/>
-    <col min="44" max="45" width="9.140625" style="10"/>
-    <col min="51" max="53" width="9.140625" style="10"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="10"/>
+    <col min="15" max="15" width="8.83203125" style="10"/>
+    <col min="21" max="21" width="8.83203125" style="10"/>
+    <col min="24" max="24" width="8.83203125" style="10"/>
+    <col min="30" max="30" width="8.83203125" style="10"/>
+    <col min="32" max="32" width="8.83203125" style="10"/>
+    <col min="36" max="36" width="8.83203125" style="10"/>
+    <col min="44" max="45" width="8.83203125" style="10"/>
+    <col min="51" max="53" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9486,7 +9498,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:53" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -9647,7 +9659,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>415</v>
       </c>
@@ -9799,7 +9811,7 @@
         <v>19597.5</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>416</v>
       </c>
@@ -9951,7 +9963,7 @@
         <v>7642.75</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>417</v>
       </c>
@@ -10103,7 +10115,7 @@
         <v>1387.25</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>418</v>
       </c>
@@ -10264,7 +10276,7 @@
         <v>18406.25</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>420</v>
       </c>
@@ -10416,7 +10428,7 @@
         <v>13369.5</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>421</v>
       </c>
@@ -10568,7 +10580,7 @@
         <v>3542.75</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>422</v>
       </c>
@@ -10720,7 +10732,7 @@
         <v>558.75</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>423</v>
       </c>
@@ -10881,7 +10893,7 @@
         <v>19160</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>424</v>
       </c>
@@ -11033,7 +11045,7 @@
         <v>14129.25</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>425</v>
       </c>
@@ -11185,7 +11197,7 @@
         <v>3496.25</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>426</v>
       </c>
@@ -11337,7 +11349,7 @@
         <v>521.5</v>
       </c>
     </row>
-    <row r="14" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>427</v>
       </c>
@@ -11498,7 +11510,7 @@
         <v>18982.75</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>428</v>
       </c>
@@ -11650,7 +11662,7 @@
         <v>13961</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>429</v>
       </c>
@@ -11802,7 +11814,7 @@
         <v>4135.25</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>430</v>
       </c>
@@ -11954,7 +11966,7 @@
         <v>615.75</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>431</v>
       </c>
@@ -12115,7 +12127,7 @@
         <v>16741.75</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>432</v>
       </c>
@@ -12267,7 +12279,7 @@
         <v>9361.25</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>433</v>
       </c>
@@ -12419,7 +12431,7 @@
         <v>2749.5</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>434</v>
       </c>
@@ -12571,7 +12583,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>435</v>
       </c>
@@ -12732,7 +12744,7 @@
         <v>17194</v>
       </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>436</v>
       </c>
@@ -12884,7 +12896,7 @@
         <v>9479</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>437</v>
       </c>
@@ -13036,7 +13048,7 @@
         <v>2638.25</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>438</v>
       </c>
@@ -13188,7 +13200,7 @@
         <v>378.25</v>
       </c>
     </row>
-    <row r="26" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>439</v>
       </c>
@@ -13349,7 +13361,7 @@
         <v>15395.5</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>440</v>
       </c>
@@ -13501,7 +13513,7 @@
         <v>9881</v>
       </c>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>441</v>
       </c>
@@ -13653,7 +13665,7 @@
         <v>2410</v>
       </c>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>442</v>
       </c>
@@ -13805,7 +13817,7 @@
         <v>328.75</v>
       </c>
     </row>
-    <row r="30" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>443</v>
       </c>
@@ -13966,7 +13978,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>444</v>
       </c>
@@ -14118,7 +14130,7 @@
         <v>12400.5</v>
       </c>
     </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>445</v>
       </c>
@@ -14270,7 +14282,7 @@
         <v>7202</v>
       </c>
     </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>446</v>
       </c>
@@ -14422,7 +14434,7 @@
         <v>1141.5</v>
       </c>
     </row>
-    <row r="34" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>447</v>
       </c>
@@ -14583,7 +14595,7 @@
         <v>17977</v>
       </c>
     </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>448</v>
       </c>
@@ -14735,7 +14747,7 @@
         <v>14146.25</v>
       </c>
     </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>449</v>
       </c>
@@ -14887,7 +14899,7 @@
         <v>5720.25</v>
       </c>
     </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>450</v>
       </c>
@@ -15039,7 +15051,7 @@
         <v>867.5</v>
       </c>
     </row>
-    <row r="38" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>451</v>
       </c>
@@ -15200,7 +15212,7 @@
         <v>17920.75</v>
       </c>
     </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>452</v>
       </c>
@@ -15352,7 +15364,7 @@
         <v>13173.25</v>
       </c>
     </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>453</v>
       </c>
@@ -15504,7 +15516,7 @@
         <v>4904.25</v>
       </c>
     </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>454</v>
       </c>
@@ -15669,12 +15681,12 @@
       <selection activeCell="AU16" sqref="AU16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:50" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15683,7 +15695,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:50" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -15835,7 +15847,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>455</v>
       </c>
@@ -15987,7 +15999,7 @@
         <v>16856.5</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>456</v>
       </c>
@@ -16139,7 +16151,7 @@
         <v>5747.75</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>457</v>
       </c>
@@ -16291,7 +16303,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>458</v>
       </c>
@@ -16443,7 +16455,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="1:50" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
         <v>459</v>
       </c>
@@ -16595,7 +16607,7 @@
         <v>16762.75</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>460</v>
       </c>
@@ -16747,7 +16759,7 @@
         <v>8305.75</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>461</v>
       </c>
@@ -16899,7 +16911,7 @@
         <v>1469.75</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>462</v>
       </c>
@@ -17064,12 +17076,12 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17080,7 +17092,7 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:53" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -17241,7 +17253,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -17393,7 +17405,7 @@
         <v>9125</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -17545,7 +17557,7 @@
         <v>16447</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -17697,7 +17709,7 @@
         <v>16163.5</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -17849,7 +17861,7 @@
         <v>8225.75</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -18001,7 +18013,7 @@
         <v>2571.25</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -18153,7 +18165,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>63</v>
       </c>
@@ -18308,7 +18320,7 @@
         <v>369.25</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>64</v>
       </c>
@@ -18469,7 +18481,7 @@
         <v>17414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -18621,7 +18633,7 @@
         <v>11238</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -18773,7 +18785,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -18925,7 +18937,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="14" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>68</v>
       </c>
@@ -19086,7 +19098,7 @@
         <v>18393</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -19238,7 +19250,7 @@
         <v>9955.75</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -19390,7 +19402,7 @@
         <v>1768.75</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -19542,7 +19554,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>72</v>
       </c>
@@ -19703,7 +19715,7 @@
         <v>12680</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -19855,7 +19867,7 @@
         <v>5566.75</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -20007,7 +20019,7 @@
         <v>780.75</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -20159,7 +20171,7 @@
         <v>93.25</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>76</v>
       </c>
@@ -20320,7 +20332,7 @@
         <v>12448</v>
       </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -20472,7 +20484,7 @@
         <v>2946.25</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -20624,7 +20636,7 @@
         <v>387.5</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -20776,7 +20788,7 @@
         <v>38.25</v>
       </c>
     </row>
-    <row r="26" spans="1:53" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>80</v>
       </c>
@@ -20937,7 +20949,7 @@
         <v>13236.25</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -21089,7 +21101,7 @@
         <v>5515.5</v>
       </c>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -21241,7 +21253,7 @@
         <v>850.5</v>
       </c>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -21393,7 +21405,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>84</v>
       </c>
@@ -21554,7 +21566,7 @@
         <v>17490.25</v>
       </c>
     </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -21706,7 +21718,7 @@
         <v>8570.5</v>
       </c>
     </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -21858,7 +21870,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -22010,7 +22022,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>88</v>
       </c>
@@ -22171,7 +22183,7 @@
         <v>14005.75</v>
       </c>
     </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -22323,7 +22335,7 @@
         <v>7813.75</v>
       </c>
     </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -22475,7 +22487,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -22627,7 +22639,7 @@
         <v>155.75</v>
       </c>
     </row>
-    <row r="38" spans="1:53" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:53" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>92</v>
       </c>
@@ -22788,7 +22800,7 @@
         <v>16514.5</v>
       </c>
     </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -22940,7 +22952,7 @@
         <v>7542.5</v>
       </c>
     </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -23092,7 +23104,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -23244,7 +23256,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>96</v>
       </c>
@@ -23405,7 +23417,7 @@
         <v>13140</v>
       </c>
     </row>
-    <row r="43" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>98</v>
       </c>
@@ -23557,7 +23569,7 @@
         <v>5471.75</v>
       </c>
     </row>
-    <row r="44" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>99</v>
       </c>
@@ -23709,7 +23721,7 @@
         <v>816.5</v>
       </c>
     </row>
-    <row r="45" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>100</v>
       </c>
@@ -23861,7 +23873,7 @@
         <v>84.5</v>
       </c>
     </row>
-    <row r="46" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>101</v>
       </c>
@@ -24022,7 +24034,7 @@
         <v>12960.75</v>
       </c>
     </row>
-    <row r="47" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>102</v>
       </c>
@@ -24174,7 +24186,7 @@
         <v>4157</v>
       </c>
     </row>
-    <row r="48" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -24326,7 +24338,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="49" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>104</v>
       </c>
@@ -24487,16 +24499,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -24510,7 +24522,7 @@
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:53" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -24671,7 +24683,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -24823,7 +24835,7 @@
         <v>17721.5</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -24975,7 +24987,7 @@
         <v>5483</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -25127,7 +25139,7 @@
         <v>881.5</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>105</v>
       </c>
@@ -25288,7 +25300,7 @@
         <v>18972.25</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -25440,7 +25452,7 @@
         <v>8873.25</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -25592,7 +25604,7 @@
         <v>1752</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -25744,7 +25756,7 @@
         <v>160.25</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>109</v>
       </c>
@@ -25905,7 +25917,7 @@
         <v>19111.5</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -26057,7 +26069,7 @@
         <v>7543.5</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>111</v>
       </c>
@@ -26209,7 +26221,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -26361,7 +26373,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:53" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>113</v>
       </c>
@@ -26522,7 +26534,7 @@
         <v>18453.25</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -26674,7 +26686,7 @@
         <v>8726</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -26826,7 +26838,7 @@
         <v>1595.5</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -26978,7 +26990,7 @@
         <v>156.75</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>117</v>
       </c>
@@ -27139,7 +27151,7 @@
         <v>17276</v>
       </c>
     </row>
-    <row r="19" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>118</v>
       </c>
@@ -27294,7 +27306,7 @@
         <v>6391.5</v>
       </c>
     </row>
-    <row r="20" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -27449,7 +27461,7 @@
         <v>987.25</v>
       </c>
     </row>
-    <row r="21" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>120</v>
       </c>
@@ -27604,7 +27616,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>121</v>
       </c>
@@ -27765,7 +27777,7 @@
         <v>17415</v>
       </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -27917,7 +27929,7 @@
         <v>6742.25</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>123</v>
       </c>
@@ -28069,7 +28081,7 @@
         <v>1057.75</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -28221,7 +28233,7 @@
         <v>93.25</v>
       </c>
     </row>
-    <row r="26" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>125</v>
       </c>
@@ -28382,7 +28394,7 @@
         <v>12152.25</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>126</v>
       </c>
@@ -28534,7 +28546,7 @@
         <v>3164.5</v>
       </c>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>127</v>
       </c>
@@ -28686,7 +28698,7 @@
         <v>405.25</v>
       </c>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>128</v>
       </c>
@@ -28838,7 +28850,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="30" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>129</v>
       </c>
@@ -28999,7 +29011,7 @@
         <v>9628.75</v>
       </c>
     </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>130</v>
       </c>
@@ -29151,7 +29163,7 @@
         <v>1754.75</v>
       </c>
     </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>131</v>
       </c>
@@ -29303,7 +29315,7 @@
         <v>233.5</v>
       </c>
     </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -29455,7 +29467,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="34" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>133</v>
       </c>
@@ -29616,7 +29628,7 @@
         <v>10058.5</v>
       </c>
     </row>
-    <row r="35" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>134</v>
       </c>
@@ -29768,7 +29780,7 @@
         <v>4766.5</v>
       </c>
     </row>
-    <row r="36" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
         <v>135</v>
       </c>
@@ -29920,7 +29932,7 @@
         <v>1110.75</v>
       </c>
     </row>
-    <row r="37" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
         <v>136</v>
       </c>
@@ -30072,7 +30084,7 @@
         <v>148.25</v>
       </c>
     </row>
-    <row r="38" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>137</v>
       </c>
@@ -30233,7 +30245,7 @@
         <v>8099.5</v>
       </c>
     </row>
-    <row r="39" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
         <v>138</v>
       </c>
@@ -30385,7 +30397,7 @@
         <v>3044.75</v>
       </c>
     </row>
-    <row r="40" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
         <v>139</v>
       </c>
@@ -30537,7 +30549,7 @@
         <v>664.5</v>
       </c>
     </row>
-    <row r="41" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
         <v>140</v>
       </c>
@@ -30689,7 +30701,7 @@
         <v>83.5</v>
       </c>
     </row>
-    <row r="42" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>141</v>
       </c>
@@ -30850,7 +30862,7 @@
         <v>16329.25</v>
       </c>
     </row>
-    <row r="43" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
         <v>142</v>
       </c>
@@ -31002,7 +31014,7 @@
         <v>12403.75</v>
       </c>
     </row>
-    <row r="44" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
         <v>143</v>
       </c>
@@ -31154,7 +31166,7 @@
         <v>4316.5</v>
       </c>
     </row>
-    <row r="45" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
         <v>144</v>
       </c>
@@ -31306,7 +31318,7 @@
         <v>598.25</v>
       </c>
     </row>
-    <row r="46" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>145</v>
       </c>
@@ -31467,7 +31479,7 @@
         <v>16361</v>
       </c>
     </row>
-    <row r="47" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>146</v>
       </c>
@@ -31619,7 +31631,7 @@
         <v>10336</v>
       </c>
     </row>
-    <row r="48" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>147</v>
       </c>
@@ -31771,7 +31783,7 @@
         <v>2331.5</v>
       </c>
     </row>
-    <row r="49" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
         <v>148</v>
       </c>
@@ -31936,19 +31948,19 @@
       <selection activeCell="E2" sqref="E2:BB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="10"/>
-    <col min="21" max="21" width="9.140625" style="10"/>
-    <col min="24" max="24" width="9.140625" style="10"/>
-    <col min="30" max="32" width="9.140625" style="10"/>
-    <col min="36" max="36" width="9.140625" style="10"/>
-    <col min="44" max="45" width="9.140625" style="10"/>
-    <col min="51" max="52" width="9.140625" style="10"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="8.83203125" style="10"/>
+    <col min="21" max="21" width="8.83203125" style="10"/>
+    <col min="24" max="24" width="8.83203125" style="10"/>
+    <col min="30" max="32" width="8.83203125" style="10"/>
+    <col min="36" max="36" width="8.83203125" style="10"/>
+    <col min="44" max="45" width="8.83203125" style="10"/>
+    <col min="51" max="52" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:55" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -31961,7 +31973,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="16"/>
     </row>
-    <row r="2" spans="1:55" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>2</v>
       </c>
@@ -32123,7 +32135,7 @@
       </c>
       <c r="BC2" s="4"/>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>8</v>
       </c>
@@ -32280,7 +32292,7 @@
       <c r="BB3" s="5"/>
       <c r="BC3" s="5"/>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
         <v>9</v>
       </c>
@@ -32437,7 +32449,7 @@
       <c r="BB4" s="5"/>
       <c r="BC4" s="5"/>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>10</v>
       </c>
@@ -32594,7 +32606,7 @@
       <c r="BB5" s="5"/>
       <c r="BC5" s="5"/>
     </row>
-    <row r="6" spans="1:55" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>149</v>
       </c>
@@ -32757,7 +32769,7 @@
       <c r="BB6" s="7"/>
       <c r="BC6" s="7"/>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>150</v>
       </c>
@@ -32914,7 +32926,7 @@
       <c r="BB7" s="5"/>
       <c r="BC7" s="5"/>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
         <v>151</v>
       </c>
@@ -33071,7 +33083,7 @@
       <c r="BB8" s="5"/>
       <c r="BC8" s="5"/>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>152</v>
       </c>
@@ -33228,7 +33240,7 @@
       <c r="BB9" s="5"/>
       <c r="BC9" s="5"/>
     </row>
-    <row r="10" spans="1:55" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
         <v>153</v>
       </c>
@@ -33391,7 +33403,7 @@
       <c r="BB10" s="9"/>
       <c r="BC10" s="9"/>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
         <v>154</v>
       </c>
@@ -33548,7 +33560,7 @@
       <c r="BB11" s="5"/>
       <c r="BC11" s="5"/>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
         <v>155</v>
       </c>
@@ -33705,7 +33717,7 @@
       <c r="BB12" s="5"/>
       <c r="BC12" s="5"/>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>156</v>
       </c>
@@ -33862,7 +33874,7 @@
       <c r="BB13" s="5"/>
       <c r="BC13" s="5"/>
     </row>
-    <row r="14" spans="1:55" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
         <v>157</v>
       </c>
@@ -34025,7 +34037,7 @@
       <c r="BB14" s="7"/>
       <c r="BC14" s="7"/>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
         <v>158</v>
       </c>
@@ -34182,7 +34194,7 @@
       <c r="BB15" s="5"/>
       <c r="BC15" s="5"/>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
         <v>159</v>
       </c>
@@ -34339,7 +34351,7 @@
       <c r="BB16" s="5"/>
       <c r="BC16" s="5"/>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
         <v>160</v>
       </c>
@@ -34496,7 +34508,7 @@
       <c r="BB17" s="5"/>
       <c r="BC17" s="5"/>
     </row>
-    <row r="18" spans="1:55" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:55" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
         <v>161</v>
       </c>
@@ -34659,7 +34671,7 @@
       <c r="BB18" s="9"/>
       <c r="BC18" s="9"/>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A19" s="24" t="s">
         <v>162</v>
       </c>
@@ -34816,7 +34828,7 @@
       <c r="BB19" s="5"/>
       <c r="BC19" s="5"/>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
         <v>163</v>
       </c>
@@ -34973,7 +34985,7 @@
       <c r="BB20" s="5"/>
       <c r="BC20" s="5"/>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
         <v>164</v>
       </c>
@@ -35130,7 +35142,7 @@
       <c r="BB21" s="5"/>
       <c r="BC21" s="5"/>
     </row>
-    <row r="22" spans="1:55" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:55" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="26" t="s">
         <v>165</v>
       </c>
@@ -35293,7 +35305,7 @@
       <c r="BB22" s="7"/>
       <c r="BC22" s="7"/>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
         <v>166</v>
       </c>
@@ -35450,7 +35462,7 @@
       <c r="BB23" s="5"/>
       <c r="BC23" s="5"/>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
         <v>167</v>
       </c>
@@ -35607,7 +35619,7 @@
       <c r="BB24" s="5"/>
       <c r="BC24" s="5"/>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
         <v>168</v>
       </c>
@@ -35764,7 +35776,7 @@
       <c r="BB25" s="5"/>
       <c r="BC25" s="5"/>
     </row>
-    <row r="26" spans="1:55" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:55" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="28" t="s">
         <v>169</v>
       </c>
@@ -35927,7 +35939,7 @@
       <c r="BB26" s="9"/>
       <c r="BC26" s="9"/>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
         <v>170</v>
       </c>
@@ -36084,7 +36096,7 @@
       <c r="BB27" s="5"/>
       <c r="BC27" s="5"/>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
         <v>171</v>
       </c>
@@ -36241,7 +36253,7 @@
       <c r="BB28" s="5"/>
       <c r="BC28" s="5"/>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A29" s="24" t="s">
         <v>172</v>
       </c>
@@ -36398,7 +36410,7 @@
       <c r="BB29" s="5"/>
       <c r="BC29" s="5"/>
     </row>
-    <row r="30" spans="1:55" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:55" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
         <v>173</v>
       </c>
@@ -36561,7 +36573,7 @@
       <c r="BB30" s="7"/>
       <c r="BC30" s="7"/>
     </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A31" s="24" t="s">
         <v>174</v>
       </c>
@@ -36718,7 +36730,7 @@
       <c r="BB31" s="5"/>
       <c r="BC31" s="5"/>
     </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A32" s="24" t="s">
         <v>175</v>
       </c>
@@ -36875,7 +36887,7 @@
       <c r="BB32" s="5"/>
       <c r="BC32" s="5"/>
     </row>
-    <row r="33" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A33" s="24" t="s">
         <v>176</v>
       </c>
@@ -37032,7 +37044,7 @@
       <c r="BB33" s="5"/>
       <c r="BC33" s="5"/>
     </row>
-    <row r="34" spans="1:55" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:55" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="28" t="s">
         <v>177</v>
       </c>
@@ -37195,7 +37207,7 @@
       <c r="BB34" s="9"/>
       <c r="BC34" s="9"/>
     </row>
-    <row r="35" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A35" s="24" t="s">
         <v>178</v>
       </c>
@@ -37352,7 +37364,7 @@
       <c r="BB35" s="5"/>
       <c r="BC35" s="5"/>
     </row>
-    <row r="36" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A36" s="24" t="s">
         <v>179</v>
       </c>
@@ -37509,7 +37521,7 @@
       <c r="BB36" s="5"/>
       <c r="BC36" s="5"/>
     </row>
-    <row r="37" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A37" s="24" t="s">
         <v>180</v>
       </c>
@@ -37666,7 +37678,7 @@
       <c r="BB37" s="5"/>
       <c r="BC37" s="5"/>
     </row>
-    <row r="38" spans="1:55" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:55" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
         <v>181</v>
       </c>
@@ -37829,7 +37841,7 @@
       <c r="BB38" s="7"/>
       <c r="BC38" s="7"/>
     </row>
-    <row r="39" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A39" s="24" t="s">
         <v>182</v>
       </c>
@@ -37986,7 +37998,7 @@
       <c r="BB39" s="5"/>
       <c r="BC39" s="5"/>
     </row>
-    <row r="40" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A40" s="24" t="s">
         <v>183</v>
       </c>
@@ -38143,7 +38155,7 @@
       <c r="BB40" s="5"/>
       <c r="BC40" s="5"/>
     </row>
-    <row r="41" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A41" s="24" t="s">
         <v>184</v>
       </c>
@@ -38300,7 +38312,7 @@
       <c r="BB41" s="5"/>
       <c r="BC41" s="5"/>
     </row>
-    <row r="42" spans="1:55" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:55" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="28" t="s">
         <v>185</v>
       </c>
@@ -38461,7 +38473,7 @@
       <c r="BB42" s="9"/>
       <c r="BC42" s="9"/>
     </row>
-    <row r="43" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A43" s="24" t="s">
         <v>187</v>
       </c>
@@ -38618,7 +38630,7 @@
       <c r="BB43" s="5"/>
       <c r="BC43" s="5"/>
     </row>
-    <row r="44" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A44" s="24" t="s">
         <v>188</v>
       </c>
@@ -38775,7 +38787,7 @@
       <c r="BB44" s="5"/>
       <c r="BC44" s="5"/>
     </row>
-    <row r="45" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A45" s="24" t="s">
         <v>189</v>
       </c>
@@ -38932,7 +38944,7 @@
       <c r="BB45" s="5"/>
       <c r="BC45" s="5"/>
     </row>
-    <row r="46" spans="1:55" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:55" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="26" t="s">
         <v>190</v>
       </c>
@@ -39093,7 +39105,7 @@
       <c r="BB46" s="7"/>
       <c r="BC46" s="7"/>
     </row>
-    <row r="47" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A47" s="24" t="s">
         <v>191</v>
       </c>
@@ -39250,7 +39262,7 @@
       <c r="BB47" s="5"/>
       <c r="BC47" s="5"/>
     </row>
-    <row r="48" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A48" s="24" t="s">
         <v>192</v>
       </c>
@@ -39407,7 +39419,7 @@
       <c r="BB48" s="5"/>
       <c r="BC48" s="5"/>
     </row>
-    <row r="49" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
         <v>193</v>
       </c>
@@ -39577,13 +39589,13 @@
       <selection activeCell="E2" sqref="E2:BB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="52" max="53" width="19.140625" customWidth="1"/>
+    <col min="52" max="53" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -39594,7 +39606,7 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:53" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -39755,7 +39767,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>194</v>
       </c>
@@ -39907,7 +39919,7 @@
         <v>17805.25</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>195</v>
       </c>
@@ -40059,7 +40071,7 @@
         <v>3790.75</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>196</v>
       </c>
@@ -40211,7 +40223,7 @@
         <v>969.75</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>197</v>
       </c>
@@ -40369,7 +40381,7 @@
         <v>16197.75</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>199</v>
       </c>
@@ -40521,7 +40533,7 @@
         <v>7838</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>200</v>
       </c>
@@ -40673,7 +40685,7 @@
         <v>2336.25</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>201</v>
       </c>
@@ -40825,7 +40837,7 @@
         <v>442.5</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>202</v>
       </c>
@@ -40986,7 +40998,7 @@
         <v>17509</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>203</v>
       </c>
@@ -41138,7 +41150,7 @@
         <v>16888</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>204</v>
       </c>
@@ -41290,7 +41302,7 @@
         <v>4711.5</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>205</v>
       </c>
@@ -41442,7 +41454,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="14" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>206</v>
       </c>
@@ -41603,7 +41615,7 @@
         <v>20221.25</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>207</v>
       </c>
@@ -41755,7 +41767,7 @@
         <v>12983.75</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>208</v>
       </c>
@@ -41907,7 +41919,7 @@
         <v>2724.25</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>209</v>
       </c>
@@ -42059,7 +42071,7 @@
         <v>301.25</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>210</v>
       </c>
@@ -42220,7 +42232,7 @@
         <v>12670.75</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>211</v>
       </c>
@@ -42372,7 +42384,7 @@
         <v>6449</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>212</v>
       </c>
@@ -42524,7 +42536,7 @@
         <v>1089.5</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>213</v>
       </c>
@@ -42676,7 +42688,7 @@
         <v>157.75</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>214</v>
       </c>
@@ -42837,7 +42849,7 @@
         <v>14755.25</v>
       </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>215</v>
       </c>
@@ -42989,7 +43001,7 @@
         <v>6759.75</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>216</v>
       </c>
@@ -43141,7 +43153,7 @@
         <v>1121.75</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>217</v>
       </c>
@@ -43293,7 +43305,7 @@
         <v>116.25</v>
       </c>
     </row>
-    <row r="26" spans="1:53" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>218</v>
       </c>
@@ -43454,7 +43466,7 @@
         <v>13055.25</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>219</v>
       </c>
@@ -43606,7 +43618,7 @@
         <v>6583.25</v>
       </c>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>220</v>
       </c>
@@ -43758,7 +43770,7 @@
         <v>1106.75</v>
       </c>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>221</v>
       </c>
@@ -43910,7 +43922,7 @@
         <v>125.25</v>
       </c>
     </row>
-    <row r="30" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>222</v>
       </c>
@@ -44071,7 +44083,7 @@
         <v>15620.25</v>
       </c>
     </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>223</v>
       </c>
@@ -44223,7 +44235,7 @@
         <v>6646.75</v>
       </c>
     </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>224</v>
       </c>
@@ -44375,7 +44387,7 @@
         <v>1001.25</v>
       </c>
     </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>225</v>
       </c>
@@ -44527,7 +44539,7 @@
         <v>107.5</v>
       </c>
     </row>
-    <row r="34" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>226</v>
       </c>
@@ -44688,7 +44700,7 @@
         <v>15270.25</v>
       </c>
     </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>227</v>
       </c>
@@ -44840,7 +44852,7 @@
         <v>8556</v>
       </c>
     </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>228</v>
       </c>
@@ -44992,7 +45004,7 @@
         <v>1319.5</v>
       </c>
     </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>229</v>
       </c>
@@ -45144,7 +45156,7 @@
         <v>129.25</v>
       </c>
     </row>
-    <row r="38" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>230</v>
       </c>
@@ -45305,7 +45317,7 @@
         <v>15631.25</v>
       </c>
     </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>231</v>
       </c>
@@ -45457,7 +45469,7 @@
         <v>6437.25</v>
       </c>
     </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>232</v>
       </c>
@@ -45609,7 +45621,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>233</v>
       </c>
@@ -45761,7 +45773,7 @@
         <v>129.75</v>
       </c>
     </row>
-    <row r="42" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>234</v>
       </c>
@@ -45922,7 +45934,7 @@
         <v>15840.25</v>
       </c>
     </row>
-    <row r="43" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>227</v>
       </c>
@@ -46074,7 +46086,7 @@
         <v>5675.25</v>
       </c>
     </row>
-    <row r="44" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>228</v>
       </c>
@@ -46226,7 +46238,7 @@
         <v>808.25</v>
       </c>
     </row>
-    <row r="45" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>229</v>
       </c>
@@ -46378,7 +46390,7 @@
         <v>85.75</v>
       </c>
     </row>
-    <row r="46" spans="1:53" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:53" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>235</v>
       </c>
@@ -46539,7 +46551,7 @@
         <v>15646.25</v>
       </c>
     </row>
-    <row r="47" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>231</v>
       </c>
@@ -46691,7 +46703,7 @@
         <v>5758</v>
       </c>
     </row>
-    <row r="48" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>232</v>
       </c>
@@ -46843,7 +46855,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="49" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>233</v>
       </c>
@@ -47008,21 +47020,21 @@
       <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="10"/>
-    <col min="15" max="15" width="9.140625" style="10"/>
-    <col min="21" max="21" width="9.140625" style="10"/>
-    <col min="24" max="24" width="9.140625" style="10"/>
-    <col min="30" max="30" width="9.140625" style="10"/>
-    <col min="32" max="32" width="9.140625" style="10"/>
-    <col min="36" max="36" width="9.140625" style="10"/>
-    <col min="44" max="45" width="9.140625" style="10"/>
-    <col min="50" max="53" width="9.140625" style="10"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="10"/>
+    <col min="15" max="15" width="8.83203125" style="10"/>
+    <col min="21" max="21" width="8.83203125" style="10"/>
+    <col min="24" max="24" width="8.83203125" style="10"/>
+    <col min="30" max="30" width="8.83203125" style="10"/>
+    <col min="32" max="32" width="8.83203125" style="10"/>
+    <col min="36" max="36" width="8.83203125" style="10"/>
+    <col min="44" max="45" width="8.83203125" style="10"/>
+    <col min="50" max="53" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -47033,7 +47045,7 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:53" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -47194,7 +47206,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -47346,7 +47358,7 @@
         <v>27231.5</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -47498,7 +47510,7 @@
         <v>9762.75</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -47650,7 +47662,7 @@
         <v>1437.5</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>236</v>
       </c>
@@ -47811,7 +47823,7 @@
         <v>33386.5</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>237</v>
       </c>
@@ -47963,7 +47975,7 @@
         <v>13530.5</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>238</v>
       </c>
@@ -48115,7 +48127,7 @@
         <v>2123.75</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -48267,7 +48279,7 @@
         <v>268.75</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>240</v>
       </c>
@@ -48428,7 +48440,7 @@
         <v>37890.5</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>241</v>
       </c>
@@ -48580,7 +48592,7 @@
         <v>13440.75</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>242</v>
       </c>
@@ -48732,7 +48744,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>243</v>
       </c>
@@ -48884,7 +48896,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>244</v>
       </c>
@@ -49045,7 +49057,7 @@
         <v>44477.5</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>245</v>
       </c>
@@ -49197,7 +49209,7 @@
         <v>14429.5</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>246</v>
       </c>
@@ -49349,7 +49361,7 @@
         <v>2679.25</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>247</v>
       </c>
@@ -49501,7 +49513,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>248</v>
       </c>
@@ -49662,7 +49674,7 @@
         <v>56539.5</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>249</v>
       </c>
@@ -49814,7 +49826,7 @@
         <v>14077.25</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>250</v>
       </c>
@@ -49966,7 +49978,7 @@
         <v>2263</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>251</v>
       </c>
@@ -50118,7 +50130,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>252</v>
       </c>
@@ -50279,7 +50291,7 @@
         <v>41734.5</v>
       </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>253</v>
       </c>
@@ -50431,7 +50443,7 @@
         <v>15747.5</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>254</v>
       </c>
@@ -50583,7 +50595,7 @@
         <v>2814.75</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>255</v>
       </c>
@@ -50735,7 +50747,7 @@
         <v>374.25</v>
       </c>
     </row>
-    <row r="26" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>256</v>
       </c>
@@ -50896,7 +50908,7 @@
         <v>31440</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>257</v>
       </c>
@@ -51048,7 +51060,7 @@
         <v>10376.25</v>
       </c>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>258</v>
       </c>
@@ -51200,7 +51212,7 @@
         <v>1618.25</v>
       </c>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>259</v>
       </c>
@@ -51352,7 +51364,7 @@
         <v>197.5</v>
       </c>
     </row>
-    <row r="30" spans="1:53" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:53" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>260</v>
       </c>
@@ -51513,7 +51525,7 @@
         <v>30240.5</v>
       </c>
     </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>261</v>
       </c>
@@ -51665,7 +51677,7 @@
         <v>14058.75</v>
       </c>
     </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>262</v>
       </c>
@@ -51817,7 +51829,7 @@
         <v>2683.5</v>
       </c>
     </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>263</v>
       </c>
@@ -51969,7 +51981,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="34" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>264</v>
       </c>
@@ -52130,7 +52142,7 @@
         <v>33047.5</v>
       </c>
     </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>265</v>
       </c>
@@ -52282,7 +52294,7 @@
         <v>13349.5</v>
       </c>
     </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>266</v>
       </c>
@@ -52434,7 +52446,7 @@
         <v>2048.75</v>
       </c>
     </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>267</v>
       </c>
@@ -52586,7 +52598,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="38" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>268</v>
       </c>
@@ -52738,7 +52750,7 @@
         <v>31795.75</v>
       </c>
     </row>
-    <row r="39" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>269</v>
       </c>
@@ -52899,7 +52911,7 @@
         <v>15304</v>
       </c>
     </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>270</v>
       </c>
@@ -53051,7 +53063,7 @@
         <v>2583.5</v>
       </c>
     </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>271</v>
       </c>
@@ -53203,7 +53215,7 @@
         <v>289.75</v>
       </c>
     </row>
-    <row r="42" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>272</v>
       </c>
@@ -53364,7 +53376,7 @@
         <v>35005</v>
       </c>
     </row>
-    <row r="43" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>273</v>
       </c>
@@ -53516,7 +53528,7 @@
         <v>12942.25</v>
       </c>
     </row>
-    <row r="44" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>274</v>
       </c>
@@ -53668,7 +53680,7 @@
         <v>2030.5</v>
       </c>
     </row>
-    <row r="45" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>275</v>
       </c>
@@ -53820,7 +53832,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="46" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>276</v>
       </c>
@@ -53981,7 +53993,7 @@
         <v>37213.5</v>
       </c>
     </row>
-    <row r="47" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>277</v>
       </c>
@@ -54133,7 +54145,7 @@
         <v>15976</v>
       </c>
     </row>
-    <row r="48" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>278</v>
       </c>
@@ -54285,7 +54297,7 @@
         <v>3104.5</v>
       </c>
     </row>
-    <row r="49" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>279</v>
       </c>
@@ -54450,12 +54462,12 @@
       <selection activeCell="E2" sqref="E2:BB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -54466,7 +54478,7 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:53" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -54627,7 +54639,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -54779,7 +54791,7 @@
         <v>19967</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -54931,7 +54943,7 @@
         <v>6860</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -55083,7 +55095,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>280</v>
       </c>
@@ -55244,7 +55256,7 @@
         <v>10406.25</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>281</v>
       </c>
@@ -55396,7 +55408,7 @@
         <v>12001.5</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>282</v>
       </c>
@@ -55548,7 +55560,7 @@
         <v>3845</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>283</v>
       </c>
@@ -55700,7 +55712,7 @@
         <v>549.5</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>284</v>
       </c>
@@ -55861,7 +55873,7 @@
         <v>26026.5</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>285</v>
       </c>
@@ -56013,7 +56025,7 @@
         <v>25696.5</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>286</v>
       </c>
@@ -56165,7 +56177,7 @@
         <v>13243.5</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>287</v>
       </c>
@@ -56317,7 +56329,7 @@
         <v>2336.75</v>
       </c>
     </row>
-    <row r="14" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>288</v>
       </c>
@@ -56478,7 +56490,7 @@
         <v>15437.5</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>289</v>
       </c>
@@ -56630,7 +56642,7 @@
         <v>18909.75</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>290</v>
       </c>
@@ -56782,7 +56794,7 @@
         <v>6958</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>291</v>
       </c>
@@ -56934,7 +56946,7 @@
         <v>1056.75</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>292</v>
       </c>
@@ -57095,7 +57107,7 @@
         <v>24119</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>293</v>
       </c>
@@ -57247,7 +57259,7 @@
         <v>23438</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>294</v>
       </c>
@@ -57399,7 +57411,7 @@
         <v>7710.75</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>295</v>
       </c>
@@ -57551,7 +57563,7 @@
         <v>1035.75</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>296</v>
       </c>
@@ -57712,7 +57724,7 @@
         <v>19684.25</v>
       </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>297</v>
       </c>
@@ -57864,7 +57876,7 @@
         <v>6591.25</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>298</v>
       </c>
@@ -58016,7 +58028,7 @@
         <v>1310.5</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>299</v>
       </c>
@@ -58168,7 +58180,7 @@
         <v>174.5</v>
       </c>
     </row>
-    <row r="26" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>300</v>
       </c>
@@ -58329,7 +58341,7 @@
         <v>22289.25</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>301</v>
       </c>
@@ -58481,7 +58493,7 @@
         <v>7709</v>
       </c>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>302</v>
       </c>
@@ -58633,7 +58645,7 @@
         <v>1090.75</v>
       </c>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>303</v>
       </c>
@@ -58785,7 +58797,7 @@
         <v>142.5</v>
       </c>
     </row>
-    <row r="30" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>304</v>
       </c>
@@ -58946,7 +58958,7 @@
         <v>12873.5</v>
       </c>
     </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>305</v>
       </c>
@@ -59098,7 +59110,7 @@
         <v>2415.75</v>
       </c>
     </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>306</v>
       </c>
@@ -59250,7 +59262,7 @@
         <v>490.25</v>
       </c>
     </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>307</v>
       </c>
@@ -59402,7 +59414,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>308</v>
       </c>
@@ -59563,7 +59575,7 @@
         <v>15126.5</v>
       </c>
     </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>309</v>
       </c>
@@ -59715,7 +59727,7 @@
         <v>3055.25</v>
       </c>
     </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>310</v>
       </c>
@@ -59867,7 +59879,7 @@
         <v>392.5</v>
       </c>
     </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>311</v>
       </c>
@@ -60019,7 +60031,7 @@
         <v>53.75</v>
       </c>
     </row>
-    <row r="38" spans="1:53" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:53" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="30" t="s">
         <v>312</v>
       </c>
@@ -60180,7 +60192,7 @@
         <v>13512.5</v>
       </c>
     </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>313</v>
       </c>
@@ -60332,7 +60344,7 @@
         <v>2512</v>
       </c>
     </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>314</v>
       </c>
@@ -60484,7 +60496,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>315</v>
       </c>
@@ -60636,7 +60648,7 @@
         <v>70.75</v>
       </c>
     </row>
-    <row r="42" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>316</v>
       </c>
@@ -60797,7 +60809,7 @@
         <v>27738</v>
       </c>
     </row>
-    <row r="43" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>318</v>
       </c>
@@ -60949,7 +60961,7 @@
         <v>12894</v>
       </c>
     </row>
-    <row r="44" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>319</v>
       </c>
@@ -61101,7 +61113,7 @@
         <v>1966.5</v>
       </c>
     </row>
-    <row r="45" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>320</v>
       </c>
@@ -61253,7 +61265,7 @@
         <v>282.5</v>
       </c>
     </row>
-    <row r="46" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>321</v>
       </c>
@@ -61414,7 +61426,7 @@
         <v>24774.75</v>
       </c>
     </row>
-    <row r="47" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>322</v>
       </c>
@@ -61566,7 +61578,7 @@
         <v>10151</v>
       </c>
     </row>
-    <row r="48" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>323</v>
       </c>
@@ -61718,7 +61730,7 @@
         <v>2313.5</v>
       </c>
     </row>
-    <row r="49" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>324</v>
       </c>
@@ -61883,20 +61895,20 @@
       <selection activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="10"/>
-    <col min="21" max="21" width="9.140625" style="10"/>
-    <col min="24" max="24" width="9.140625" style="10"/>
-    <col min="30" max="30" width="9.140625" style="10"/>
-    <col min="32" max="32" width="9.140625" style="10"/>
-    <col min="36" max="36" width="9.140625" style="10"/>
-    <col min="44" max="45" width="9.140625" style="10"/>
-    <col min="50" max="53" width="9.140625" style="10"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="10"/>
+    <col min="21" max="21" width="8.83203125" style="10"/>
+    <col min="24" max="24" width="8.83203125" style="10"/>
+    <col min="30" max="30" width="8.83203125" style="10"/>
+    <col min="32" max="32" width="8.83203125" style="10"/>
+    <col min="36" max="36" width="8.83203125" style="10"/>
+    <col min="44" max="45" width="8.83203125" style="10"/>
+    <col min="50" max="53" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -61909,7 +61921,7 @@
       <c r="AD1" s="22"/>
       <c r="AE1" s="10"/>
     </row>
-    <row r="2" spans="1:53" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -62070,7 +62082,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -62222,7 +62234,7 @@
         <v>16102.25</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -62374,7 +62386,7 @@
         <v>5417.25</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -62526,7 +62538,7 @@
         <v>505.75</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>325</v>
       </c>
@@ -62687,7 +62699,7 @@
         <v>13148.25</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>326</v>
       </c>
@@ -62839,7 +62851,7 @@
         <v>19306</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>327</v>
       </c>
@@ -62991,7 +63003,7 @@
         <v>9378</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>328</v>
       </c>
@@ -63143,7 +63155,7 @@
         <v>1861.25</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>329</v>
       </c>
@@ -63304,7 +63316,7 @@
         <v>10404.25</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>330</v>
       </c>
@@ -63456,7 +63468,7 @@
         <v>28696.75</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>331</v>
       </c>
@@ -63608,7 +63620,7 @@
         <v>20954.5</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>332</v>
       </c>
@@ -63760,7 +63772,7 @@
         <v>8695.75</v>
       </c>
     </row>
-    <row r="14" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>333</v>
       </c>
@@ -63921,7 +63933,7 @@
         <v>13459.5</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>334</v>
       </c>
@@ -64073,7 +64085,7 @@
         <v>2933</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>335</v>
       </c>
@@ -64225,7 +64237,7 @@
         <v>513.75</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>336</v>
       </c>
@@ -64377,7 +64389,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>337</v>
       </c>
@@ -64538,7 +64550,7 @@
         <v>10229</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>338</v>
       </c>
@@ -64690,7 +64702,7 @@
         <v>4013.25</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>339</v>
       </c>
@@ -64842,7 +64854,7 @@
         <v>561.5</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>340</v>
       </c>
@@ -64994,7 +65006,7 @@
         <v>80.25</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>341</v>
       </c>
@@ -65155,7 +65167,7 @@
         <v>11717.75</v>
       </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>342</v>
       </c>
@@ -65307,7 +65319,7 @@
         <v>6855.5</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>343</v>
       </c>
@@ -65459,7 +65471,7 @@
         <v>1513.75</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>344</v>
       </c>
@@ -65611,7 +65623,7 @@
         <v>276.25</v>
       </c>
     </row>
-    <row r="26" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>345</v>
       </c>
@@ -65772,7 +65784,7 @@
         <v>7465.5</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>346</v>
       </c>
@@ -65924,7 +65936,7 @@
         <v>7315.5</v>
       </c>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>347</v>
       </c>
@@ -66076,7 +66088,7 @@
         <v>3030.25</v>
       </c>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>348</v>
       </c>
@@ -66228,7 +66240,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="30" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>349</v>
       </c>
@@ -66389,7 +66401,7 @@
         <v>7458.5</v>
       </c>
     </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>350</v>
       </c>
@@ -66541,7 +66553,7 @@
         <v>1651.75</v>
       </c>
     </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>351</v>
       </c>
@@ -66693,7 +66705,7 @@
         <v>217.75</v>
       </c>
     </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>352</v>
       </c>
@@ -66845,7 +66857,7 @@
         <v>35.75</v>
       </c>
     </row>
-    <row r="34" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>353</v>
       </c>
@@ -67006,7 +67018,7 @@
         <v>5185</v>
       </c>
     </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>354</v>
       </c>
@@ -67158,7 +67170,7 @@
         <v>5245.75</v>
       </c>
     </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>355</v>
       </c>
@@ -67310,7 +67322,7 @@
         <v>891.75</v>
       </c>
     </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>356</v>
       </c>
@@ -67462,7 +67474,7 @@
         <v>147.75</v>
       </c>
     </row>
-    <row r="38" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>357</v>
       </c>
@@ -67623,7 +67635,7 @@
         <v>53.75</v>
       </c>
     </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>358</v>
       </c>
@@ -67775,7 +67787,7 @@
         <v>29.25</v>
       </c>
     </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>359</v>
       </c>
@@ -67927,7 +67939,7 @@
         <v>16.75</v>
       </c>
     </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>360</v>
       </c>
@@ -68079,7 +68091,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="42" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>361</v>
       </c>
@@ -68240,7 +68252,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>362</v>
       </c>
@@ -68392,7 +68404,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>363</v>
       </c>
@@ -68544,7 +68556,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="45" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>364</v>
       </c>
@@ -68696,7 +68708,7 @@
         <v>16.25</v>
       </c>
     </row>
-    <row r="46" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>365</v>
       </c>
@@ -68857,7 +68869,7 @@
         <v>17778.5</v>
       </c>
     </row>
-    <row r="47" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>367</v>
       </c>
@@ -69009,7 +69021,7 @@
         <v>11277.25</v>
       </c>
     </row>
-    <row r="48" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>368</v>
       </c>
@@ -69161,7 +69173,7 @@
         <v>2279.75</v>
       </c>
     </row>
-    <row r="49" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>369</v>
       </c>
@@ -69326,21 +69338,21 @@
       <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="10"/>
-    <col min="21" max="21" width="9.140625" style="10"/>
-    <col min="24" max="24" width="9.140625" style="10"/>
-    <col min="30" max="30" width="9.140625" style="10"/>
-    <col min="32" max="32" width="9.140625" style="10"/>
-    <col min="36" max="36" width="9.140625" style="10"/>
-    <col min="44" max="45" width="9.140625" style="10"/>
-    <col min="50" max="51" width="9.140625" style="10"/>
-    <col min="53" max="53" width="9.140625" style="10"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="10"/>
+    <col min="21" max="21" width="8.83203125" style="10"/>
+    <col min="24" max="24" width="8.83203125" style="10"/>
+    <col min="30" max="30" width="8.83203125" style="10"/>
+    <col min="32" max="32" width="8.83203125" style="10"/>
+    <col min="36" max="36" width="8.83203125" style="10"/>
+    <col min="44" max="45" width="8.83203125" style="10"/>
+    <col min="50" max="51" width="8.83203125" style="10"/>
+    <col min="53" max="53" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -69352,7 +69364,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:53" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -69513,7 +69525,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -69665,7 +69677,7 @@
         <v>9771.75</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -69817,7 +69829,7 @@
         <v>4669</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -69969,7 +69981,7 @@
         <v>691.5</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>370</v>
       </c>
@@ -70130,7 +70142,7 @@
         <v>10718.5</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>371</v>
       </c>
@@ -70282,7 +70294,7 @@
         <v>9800.5</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>372</v>
       </c>
@@ -70434,7 +70446,7 @@
         <v>1958.75</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>373</v>
       </c>
@@ -70586,7 +70598,7 @@
         <v>251.75</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>374</v>
       </c>
@@ -70747,7 +70759,7 @@
         <v>9335.5</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>375</v>
       </c>
@@ -70899,7 +70911,7 @@
         <v>7577</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>376</v>
       </c>
@@ -71051,7 +71063,7 @@
         <v>1521</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>377</v>
       </c>
@@ -71203,7 +71215,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="14" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>378</v>
       </c>
@@ -71364,7 +71376,7 @@
         <v>13203.75</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>379</v>
       </c>
@@ -71516,7 +71528,7 @@
         <v>9784.5</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>380</v>
       </c>
@@ -71668,7 +71680,7 @@
         <v>2532.25</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>381</v>
       </c>
@@ -71820,7 +71832,7 @@
         <v>370.25</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>382</v>
       </c>
@@ -71981,7 +71993,7 @@
         <v>6788.5</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>383</v>
       </c>
@@ -72133,7 +72145,7 @@
         <v>5624</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>384</v>
       </c>
@@ -72285,7 +72297,7 @@
         <v>921.5</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>385</v>
       </c>
@@ -72437,7 +72449,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>386</v>
       </c>
@@ -72598,7 +72610,7 @@
         <v>7618.5</v>
       </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>387</v>
       </c>
@@ -72750,7 +72762,7 @@
         <v>4994.75</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>388</v>
       </c>
@@ -72902,7 +72914,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>389</v>
       </c>
@@ -73054,7 +73066,7 @@
         <v>125.5</v>
       </c>
     </row>
-    <row r="26" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>390</v>
       </c>
@@ -73215,7 +73227,7 @@
         <v>6646.75</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>391</v>
       </c>
@@ -73367,7 +73379,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>392</v>
       </c>
@@ -73519,7 +73531,7 @@
         <v>381.5</v>
       </c>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>393</v>
       </c>
@@ -73671,7 +73683,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>394</v>
       </c>
@@ -73832,7 +73844,7 @@
         <v>5679.5</v>
       </c>
     </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>395</v>
       </c>
@@ -73984,7 +73996,7 @@
         <v>2488.25</v>
       </c>
     </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>396</v>
       </c>
@@ -74136,7 +74148,7 @@
         <v>321.25</v>
       </c>
     </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>397</v>
       </c>
@@ -74288,7 +74300,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>398</v>
       </c>
@@ -74443,7 +74455,7 @@
         <v>4871.5</v>
       </c>
     </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>400</v>
       </c>
@@ -74595,7 +74607,7 @@
         <v>3356.25</v>
       </c>
     </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>401</v>
       </c>
@@ -74747,7 +74759,7 @@
         <v>675.25</v>
       </c>
     </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>402</v>
       </c>
@@ -74899,7 +74911,7 @@
         <v>81.75</v>
       </c>
     </row>
-    <row r="38" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>403</v>
       </c>
@@ -75054,7 +75066,7 @@
         <v>9588.25</v>
       </c>
     </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>404</v>
       </c>
@@ -75206,7 +75218,7 @@
         <v>3523</v>
       </c>
     </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>405</v>
       </c>
@@ -75358,7 +75370,7 @@
         <v>582.25</v>
       </c>
     </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>406</v>
       </c>
@@ -75510,7 +75522,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:53" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>407</v>
       </c>
@@ -75665,7 +75677,7 @@
         <v>4964</v>
       </c>
     </row>
-    <row r="43" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>408</v>
       </c>
@@ -75817,7 +75829,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="44" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>409</v>
       </c>
@@ -75969,7 +75981,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="45" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>410</v>
       </c>
@@ -76121,7 +76133,7 @@
         <v>39.75</v>
       </c>
     </row>
-    <row r="46" spans="1:53" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:53" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>411</v>
       </c>
@@ -76276,7 +76288,7 @@
         <v>6870</v>
       </c>
     </row>
-    <row r="47" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>412</v>
       </c>
@@ -76428,7 +76440,7 @@
         <v>3697</v>
       </c>
     </row>
-    <row r="48" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>413</v>
       </c>
@@ -76580,7 +76592,7 @@
         <v>716.5</v>
       </c>
     </row>
-    <row r="49" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>414</v>
       </c>

</xml_diff>

<commit_message>
now saves a csv of the reformatted data frame.
</commit_message>
<xml_diff>
--- a/Assignment4/06222016 Staph Array Data.xlsx
+++ b/Assignment4/06222016 Staph Array Data.xlsx
@@ -2028,7 +2028,7 @@
   <dimension ref="A1:BB49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17072,7 +17072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA49"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -31944,7 +31944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:BB2"/>
     </sheetView>
   </sheetViews>
@@ -39585,7 +39585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA49"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:BB2"/>
     </sheetView>
   </sheetViews>
@@ -47016,7 +47016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA49"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>

</xml_diff>